<commit_message>
Updated all motor A, B and Dir pins. Updated pinout file.
</commit_message>
<xml_diff>
--- a/direcs-arduino/omnibot/pinout.xlsx
+++ b/direcs-arduino/omnibot/pinout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25711"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="203">
   <si>
     <t>Pin Number</t>
   </si>
@@ -594,6 +594,45 @@
   </si>
   <si>
     <t>motor4PWMPin</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>motor1aPin</t>
+  </si>
+  <si>
+    <t>motor1bPin</t>
+  </si>
+  <si>
+    <t>motor1DirPin</t>
+  </si>
+  <si>
+    <t>motor2aPin</t>
+  </si>
+  <si>
+    <t>motor2bPin</t>
+  </si>
+  <si>
+    <t>motor2DirPin</t>
+  </si>
+  <si>
+    <t>motor3aPin</t>
+  </si>
+  <si>
+    <t>motor3bPin</t>
+  </si>
+  <si>
+    <t>motor3DirPin</t>
+  </si>
+  <si>
+    <t>motor4aPin</t>
+  </si>
+  <si>
+    <t>motor4bPin</t>
+  </si>
+  <si>
+    <t>motor4DirPin</t>
   </si>
 </sst>
 </file>
@@ -609,7 +648,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -619,6 +658,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -635,12 +680,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -922,20 +973,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -945,11 +997,20 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>97</v>
       </c>
@@ -960,7 +1021,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>96</v>
       </c>
@@ -971,7 +1032,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>87</v>
       </c>
@@ -982,7 +1043,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>86</v>
       </c>
@@ -993,7 +1054,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>85</v>
       </c>
@@ -1004,7 +1065,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>84</v>
       </c>
@@ -1015,7 +1076,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>83</v>
       </c>
@@ -1026,7 +1087,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>82</v>
       </c>
@@ -1037,7 +1098,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>95</v>
       </c>
@@ -1048,7 +1109,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>94</v>
       </c>
@@ -1059,7 +1120,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>93</v>
       </c>
@@ -1070,7 +1131,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>92</v>
       </c>
@@ -1081,7 +1142,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>91</v>
       </c>
@@ -1092,7 +1153,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>90</v>
       </c>
@@ -1103,7 +1164,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>89</v>
       </c>
@@ -1136,7 +1197,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -1146,8 +1207,20 @@
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D19" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -1156,6 +1229,18 @@
       </c>
       <c r="C20" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1325,7 +1410,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>78</v>
       </c>
@@ -1335,8 +1420,11 @@
       <c r="C34" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D34" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>77</v>
       </c>
@@ -1346,8 +1434,11 @@
       <c r="C35" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D35" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>76</v>
       </c>
@@ -1357,8 +1448,11 @@
       <c r="C36" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D36" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>75</v>
       </c>
@@ -1368,8 +1462,11 @@
       <c r="C37" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D37" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>74</v>
       </c>
@@ -1379,8 +1476,11 @@
       <c r="C38" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D38" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>73</v>
       </c>
@@ -1390,8 +1490,11 @@
       <c r="C39" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D39" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>72</v>
       </c>
@@ -1401,8 +1504,11 @@
       <c r="C40" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D40" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>71</v>
       </c>
@@ -1411,6 +1517,9 @@
       </c>
       <c r="C41" s="1" t="s">
         <v>116</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1430,7 +1539,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>60</v>
       </c>
@@ -1440,8 +1549,11 @@
       <c r="C43" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D43" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>59</v>
       </c>
@@ -1451,8 +1563,11 @@
       <c r="C44" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D44" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>58</v>
       </c>
@@ -1462,8 +1577,11 @@
       <c r="C45" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D45" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>57</v>
       </c>
@@ -1472,6 +1590,9 @@
       </c>
       <c r="C46" s="1" t="s">
         <v>97</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1507,7 +1628,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>53</v>
       </c>
@@ -1518,7 +1639,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1529,7 +1650,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>70</v>
       </c>
@@ -1540,7 +1661,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>1</v>
       </c>
@@ -1557,7 +1678,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1568,7 +1689,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>51</v>
       </c>
@@ -1579,7 +1700,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>42</v>
       </c>
@@ -1590,7 +1711,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>41</v>
       </c>
@@ -1601,7 +1722,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>40</v>
       </c>
@@ -1612,7 +1733,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>39</v>
       </c>
@@ -1623,7 +1744,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>38</v>
       </c>
@@ -1634,7 +1755,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>37</v>
       </c>
@@ -1645,7 +1766,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>36</v>
       </c>
@@ -1656,7 +1777,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>35</v>
       </c>
@@ -1667,7 +1788,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>5</v>
       </c>
@@ -1684,7 +1805,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>22</v>
       </c>
@@ -1695,7 +1816,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>21</v>
       </c>
@@ -1706,7 +1827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>20</v>
       </c>
@@ -1717,7 +1838,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>19</v>
       </c>
@@ -1728,7 +1849,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>15</v>
       </c>
@@ -1745,7 +1866,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>16</v>
       </c>
@@ -1762,7 +1883,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>17</v>
       </c>
@@ -1779,7 +1900,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>18</v>
       </c>
@@ -1796,7 +1917,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>11</v>
       </c>
@@ -1807,7 +1928,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>32</v>
       </c>
@@ -1818,7 +1939,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>62</v>
       </c>
@@ -1829,7 +1950,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>81</v>
       </c>
@@ -1840,7 +1961,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>99</v>
       </c>
@@ -1851,7 +1972,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>30</v>
       </c>
@@ -1862,7 +1983,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>10</v>
       </c>
@@ -1873,7 +1994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>31</v>
       </c>
@@ -1884,7 +2005,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>61</v>
       </c>
@@ -1895,7 +2016,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1906,7 +2027,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>100</v>
       </c>
@@ -1917,7 +2038,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>34</v>
       </c>
@@ -1928,7 +2049,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>33</v>
       </c>
@@ -1939,7 +2060,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>4</v>
       </c>
@@ -1947,7 +2068,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>8</v>
       </c>
@@ -1955,7 +2076,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>9</v>
       </c>
@@ -1963,7 +2084,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>14</v>
       </c>
@@ -1971,7 +2092,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>27</v>
       </c>
@@ -1979,7 +2100,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>28</v>
       </c>
@@ -1987,7 +2108,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>29</v>
       </c>
@@ -1995,7 +2116,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>47</v>
       </c>
@@ -2003,7 +2124,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>48</v>
       </c>
@@ -2011,7 +2132,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>49</v>
       </c>
@@ -2019,7 +2140,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>65</v>
       </c>
@@ -2027,7 +2148,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>66</v>
       </c>
@@ -2035,7 +2156,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>67</v>
       </c>
@@ -2043,7 +2164,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>68</v>
       </c>
@@ -2051,7 +2172,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>69</v>
       </c>
@@ -2059,7 +2180,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>79</v>
       </c>

</xml_diff>

<commit_message>
Updated _all_ pins in omnibot.
</commit_message>
<xml_diff>
--- a/direcs-arduino/omnibot/pinout.xlsx
+++ b/direcs-arduino/omnibot/pinout.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25908"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25823"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markus/develop/direcs/direcs-arduino/omnibot/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="15360" tabRatio="500"/>
+    <workbookView xWindow="8300" yWindow="0" windowWidth="41080" windowHeight="25580" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Tabelle1!$A$1:$G$101</definedName>
+  </definedNames>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="213">
   <si>
     <t>Pin Number</t>
   </si>
@@ -633,16 +631,68 @@
   </si>
   <si>
     <t>motor4DirPin</t>
+  </si>
+  <si>
+    <t>SPARE</t>
+  </si>
+  <si>
+    <t>ledRed</t>
+  </si>
+  <si>
+    <t>ledGreen</t>
+  </si>
+  <si>
+    <t>ledYellow</t>
+  </si>
+  <si>
+    <t>relaisPin</t>
+  </si>
+  <si>
+    <t>IR_Rcv_PIN</t>
+  </si>
+  <si>
+    <t>analogInPin</t>
+  </si>
+  <si>
+    <t>FONA_RX</t>
+  </si>
+  <si>
+    <t>FONA_TX</t>
+  </si>
+  <si>
+    <t>FONA_RST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -677,8 +727,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -695,8 +755,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+  <cellStyles count="11">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -751,7 +821,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -786,7 +856,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -963,7 +1033,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -971,14 +1041,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="1"/>
     <col min="2" max="2" width="23.1640625" style="1" bestFit="1" customWidth="1"/>
@@ -987,7 +1060,7 @@
     <col min="5" max="7" width="14.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1083,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>97</v>
       </c>
@@ -1020,8 +1093,11 @@
       <c r="C2" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D2" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>96</v>
       </c>
@@ -1032,7 +1108,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>87</v>
       </c>
@@ -1043,7 +1119,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>86</v>
       </c>
@@ -1054,7 +1130,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>85</v>
       </c>
@@ -1065,7 +1141,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>84</v>
       </c>
@@ -1076,7 +1152,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>83</v>
       </c>
@@ -1087,7 +1163,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>82</v>
       </c>
@@ -1098,7 +1174,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>95</v>
       </c>
@@ -1109,7 +1185,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>94</v>
       </c>
@@ -1120,7 +1196,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>93</v>
       </c>
@@ -1131,7 +1207,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>92</v>
       </c>
@@ -1142,7 +1218,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>91</v>
       </c>
@@ -1153,7 +1229,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>90</v>
       </c>
@@ -1164,7 +1240,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>89</v>
       </c>
@@ -1175,7 +1251,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>88</v>
       </c>
@@ -1186,7 +1262,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>98</v>
       </c>
@@ -1197,7 +1273,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -1220,7 +1296,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -1243,7 +1319,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>23</v>
       </c>
@@ -1260,7 +1336,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>24</v>
       </c>
@@ -1277,7 +1353,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>25</v>
       </c>
@@ -1288,7 +1364,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>26</v>
       </c>
@@ -1299,7 +1375,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>64</v>
       </c>
@@ -1310,7 +1386,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>63</v>
       </c>
@@ -1321,7 +1397,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>13</v>
       </c>
@@ -1331,8 +1407,11 @@
       <c r="C27" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D27" s="1" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>12</v>
       </c>
@@ -1342,8 +1421,11 @@
       <c r="C28" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D28" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>46</v>
       </c>
@@ -1353,8 +1435,11 @@
       <c r="C29" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D29" s="1" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>45</v>
       </c>
@@ -1365,7 +1450,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>6</v>
       </c>
@@ -1388,7 +1473,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>44</v>
       </c>
@@ -1399,7 +1484,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>43</v>
       </c>
@@ -1410,7 +1495,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>78</v>
       </c>
@@ -1424,7 +1509,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>77</v>
       </c>
@@ -1438,7 +1523,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>76</v>
       </c>
@@ -1452,7 +1537,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>75</v>
       </c>
@@ -1466,7 +1551,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>74</v>
       </c>
@@ -1480,7 +1565,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>73</v>
       </c>
@@ -1494,7 +1579,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>72</v>
       </c>
@@ -1508,7 +1593,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>71</v>
       </c>
@@ -1522,7 +1607,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>7</v>
       </c>
@@ -1539,7 +1624,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>60</v>
       </c>
@@ -1553,7 +1638,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>59</v>
       </c>
@@ -1567,7 +1652,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>58</v>
       </c>
@@ -1581,7 +1666,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>57</v>
       </c>
@@ -1595,7 +1680,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>56</v>
       </c>
@@ -1605,8 +1690,11 @@
       <c r="C47" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D47" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>55</v>
       </c>
@@ -1616,8 +1704,11 @@
       <c r="C48" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D48" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1">
         <v>54</v>
       </c>
@@ -1627,8 +1718,11 @@
       <c r="C49" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D49" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1">
         <v>53</v>
       </c>
@@ -1638,8 +1732,11 @@
       <c r="C50" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -1649,8 +1746,11 @@
       <c r="C51" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D51" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1">
         <v>70</v>
       </c>
@@ -1661,7 +1761,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7">
       <c r="A53" s="1">
         <v>1</v>
       </c>
@@ -1678,7 +1778,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1689,7 +1789,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7">
       <c r="A55" s="1">
         <v>51</v>
       </c>
@@ -1700,7 +1800,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7">
       <c r="A56" s="1">
         <v>42</v>
       </c>
@@ -1710,8 +1810,20 @@
       <c r="C56" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D56" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1">
         <v>41</v>
       </c>
@@ -1722,7 +1834,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7">
       <c r="A58" s="1">
         <v>40</v>
       </c>
@@ -1733,7 +1845,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7">
       <c r="A59" s="1">
         <v>39</v>
       </c>
@@ -1744,7 +1856,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7">
       <c r="A60" s="1">
         <v>38</v>
       </c>
@@ -1755,7 +1867,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7">
       <c r="A61" s="1">
         <v>37</v>
       </c>
@@ -1766,7 +1878,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7">
       <c r="A62" s="1">
         <v>36</v>
       </c>
@@ -1777,7 +1889,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7">
       <c r="A63" s="1">
         <v>35</v>
       </c>
@@ -1788,7 +1900,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7">
       <c r="A64" s="1">
         <v>5</v>
       </c>
@@ -1805,7 +1917,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5">
       <c r="A65" s="1">
         <v>22</v>
       </c>
@@ -1816,7 +1928,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5">
       <c r="A66" s="1">
         <v>21</v>
       </c>
@@ -1827,7 +1939,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5">
       <c r="A67" s="1">
         <v>20</v>
       </c>
@@ -1838,7 +1950,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5">
       <c r="A68" s="1">
         <v>19</v>
       </c>
@@ -1849,7 +1961,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5">
       <c r="A69" s="1">
         <v>15</v>
       </c>
@@ -1866,7 +1978,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5">
       <c r="A70" s="1">
         <v>16</v>
       </c>
@@ -1883,7 +1995,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5">
       <c r="A71" s="1">
         <v>17</v>
       </c>
@@ -1900,7 +2012,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5">
       <c r="A72" s="1">
         <v>18</v>
       </c>
@@ -1917,7 +2029,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5">
       <c r="A73" s="1">
         <v>11</v>
       </c>
@@ -1928,7 +2040,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5">
       <c r="A74" s="1">
         <v>32</v>
       </c>
@@ -1939,7 +2051,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5">
       <c r="A75" s="1">
         <v>62</v>
       </c>
@@ -1950,7 +2062,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5">
       <c r="A76" s="1">
         <v>81</v>
       </c>
@@ -1961,7 +2073,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5">
       <c r="A77" s="1">
         <v>99</v>
       </c>
@@ -1972,7 +2084,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5">
       <c r="A78" s="1">
         <v>30</v>
       </c>
@@ -1983,7 +2095,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5">
       <c r="A79" s="1">
         <v>10</v>
       </c>
@@ -1994,7 +2106,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5">
       <c r="A80" s="1">
         <v>31</v>
       </c>
@@ -2005,7 +2117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3">
       <c r="A81" s="1">
         <v>61</v>
       </c>
@@ -2016,7 +2128,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2027,7 +2139,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3">
       <c r="A83" s="1">
         <v>100</v>
       </c>
@@ -2038,7 +2150,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3">
       <c r="A84" s="1">
         <v>34</v>
       </c>
@@ -2049,7 +2161,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3">
       <c r="A85" s="1">
         <v>33</v>
       </c>
@@ -2060,7 +2172,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3">
       <c r="A86" s="1">
         <v>4</v>
       </c>
@@ -2068,7 +2180,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3">
       <c r="A87" s="1">
         <v>8</v>
       </c>
@@ -2076,7 +2188,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3">
       <c r="A88" s="1">
         <v>9</v>
       </c>
@@ -2084,7 +2196,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3">
       <c r="A89" s="1">
         <v>14</v>
       </c>
@@ -2092,7 +2204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3">
       <c r="A90" s="1">
         <v>27</v>
       </c>
@@ -2100,7 +2212,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3">
       <c r="A91" s="1">
         <v>28</v>
       </c>
@@ -2108,7 +2220,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3">
       <c r="A92" s="1">
         <v>29</v>
       </c>
@@ -2116,7 +2228,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3">
       <c r="A93" s="1">
         <v>47</v>
       </c>
@@ -2124,7 +2236,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3">
       <c r="A94" s="1">
         <v>48</v>
       </c>
@@ -2132,7 +2244,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3">
       <c r="A95" s="1">
         <v>49</v>
       </c>
@@ -2140,7 +2252,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3">
       <c r="A96" s="1">
         <v>65</v>
       </c>
@@ -2148,7 +2260,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2">
       <c r="A97" s="1">
         <v>66</v>
       </c>
@@ -2156,7 +2268,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98" s="1">
         <v>67</v>
       </c>
@@ -2164,7 +2276,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2">
       <c r="A99" s="1">
         <v>68</v>
       </c>
@@ -2172,7 +2284,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2">
       <c r="A100" s="1">
         <v>69</v>
       </c>
@@ -2180,7 +2292,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2">
       <c r="A101" s="1">
         <v>79</v>
       </c>
@@ -2192,6 +2304,13 @@
   <sortState ref="A2:C101">
     <sortCondition ref="C2:C101"/>
   </sortState>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="47" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Removed motorNDirPin and their setup. Not needed for Monster Moto Shield. Added setMotorSpeed function.
</commit_message>
<xml_diff>
--- a/direcs-arduino/omnibot/pinout.xlsx
+++ b/direcs-arduino/omnibot/pinout.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="209">
   <si>
     <t>Pin Number</t>
   </si>
@@ -608,34 +608,22 @@
     <t>motor1bPin</t>
   </si>
   <si>
-    <t>motor1DirPin</t>
-  </si>
-  <si>
     <t>motor2aPin</t>
   </si>
   <si>
     <t>motor2bPin</t>
   </si>
   <si>
-    <t>motor2DirPin</t>
-  </si>
-  <si>
     <t>motor3aPin</t>
   </si>
   <si>
     <t>motor3bPin</t>
   </si>
   <si>
-    <t>motor3DirPin</t>
-  </si>
-  <si>
     <t>motor4aPin</t>
   </si>
   <si>
     <t>motor4bPin</t>
-  </si>
-  <si>
-    <t>motor4DirPin</t>
   </si>
   <si>
     <t>SPARE</t>
@@ -1070,9 +1058,9 @@
   </sheetPr>
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="131" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1106,7 @@
         <v>163</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -1519,7 +1507,7 @@
         <v>23</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1536,7 +1524,7 @@
         <v>21</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1553,7 +1541,7 @@
         <v>78</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -1671,9 +1659,7 @@
       <c r="C36" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D36" s="4" t="s">
-        <v>193</v>
-      </c>
+      <c r="D36" s="4"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -1689,7 +1675,7 @@
         <v>124</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -1706,7 +1692,7 @@
         <v>122</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -1722,9 +1708,7 @@
       <c r="C39" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>196</v>
-      </c>
+      <c r="D39" s="4"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -1740,7 +1724,7 @@
         <v>118</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -1757,7 +1741,7 @@
         <v>116</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -1792,9 +1776,7 @@
       <c r="C43" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>199</v>
-      </c>
+      <c r="D43" s="4"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -1810,7 +1792,7 @@
         <v>101</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -1827,7 +1809,7 @@
         <v>99</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -1843,9 +1825,7 @@
       <c r="C46" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D46" s="4" t="s">
-        <v>202</v>
-      </c>
+      <c r="D46" s="4"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
@@ -1861,7 +1841,7 @@
         <v>95</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -1878,7 +1858,7 @@
         <v>93</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -1895,7 +1875,7 @@
         <v>91</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -1912,7 +1892,7 @@
         <v>89</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -1929,7 +1909,7 @@
         <v>83</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -2010,16 +1990,16 @@
         <v>70</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed motor pins due to not needed motorDirPins.
</commit_message>
<xml_diff>
--- a/direcs-arduino/omnibot/pinout.xlsx
+++ b/direcs-arduino/omnibot/pinout.xlsx
@@ -1059,8 +1059,8 @@
   <dimension ref="A1:G101"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="131" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -1659,7 +1659,9 @@
       <c r="C36" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="D36" s="4"/>
+      <c r="D36" s="4" t="s">
+        <v>193</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -1675,7 +1677,7 @@
         <v>124</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -1692,7 +1694,7 @@
         <v>122</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -1708,7 +1710,9 @@
       <c r="C39" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -1724,7 +1728,7 @@
         <v>118</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -1741,7 +1745,7 @@
         <v>116</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -1791,9 +1795,7 @@
       <c r="C44" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D44" s="4" t="s">
-        <v>197</v>
-      </c>
+      <c r="D44" s="4"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
@@ -1808,9 +1810,7 @@
       <c r="C45" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D45" s="4" t="s">
-        <v>198</v>
-      </c>
+      <c r="D45" s="4"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>

</xml_diff>